<commit_message>
added code to format the numeric value from Excel to string
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/testData.xlsx
+++ b/src/test/java/TestData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationClasses\2025\Group5-2025\SeleniumJava5thGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C0E41C-1822-456B-8045-2A7C130F8D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C377B3EF-1C6E-4F57-B07B-83792D5B11B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29985" yWindow="630" windowWidth="9480" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Username</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>invadi@email.com</t>
-  </si>
-  <si>
-    <t>12345678</t>
   </si>
   <si>
     <t>#123ew4567dsf8w</t>
@@ -108,12 +105,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -398,20 +398,20 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -419,29 +419,29 @@
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
+      <c r="B3" s="5">
+        <v>12345678</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="B6" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added different examples to write to an Excel file
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/testData.xlsx
+++ b/src/test/java/TestData/testData.xlsx
@@ -1,31 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationClasses\2025\Group5-2025\SeleniumJava5thGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C377B3EF-1C6E-4F57-B07B-83792D5B11B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2C4B65-E2D8-473A-ACB3-C574914422F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Employees" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Legal</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
   <si>
     <t>Username</t>
   </si>
@@ -36,20 +59,30 @@
     <t>sbuda@gmail.com</t>
   </si>
   <si>
-    <t>invadi@email.com</t>
-  </si>
-  <si>
-    <t>#123ew4567dsf8w</t>
+    <t>password1</t>
+  </si>
+  <si>
+    <t>Diana</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Dion</t>
+  </si>
+  <si>
+    <t>Operations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,15 +138,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -149,7 +178,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -161,7 +190,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -208,6 +237,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -243,6 +289,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -395,58 +458,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="2.6328125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.54296875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7265625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD02E658-6D3E-449E-8143-7745BC394AC4}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.36328125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.90625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3">
         <v>12345678</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{C747CFC0-A0F6-453B-AD87-2731937B4CE8}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{785BA305-1B03-4D6A-BAA1-2323F05F595C}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C525BEF0-D523-400F-A5C2-8C971B718019}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{1AAF99F9-B742-4F3A-A2C9-BD1FA5D7D1B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
called DataFormatter class to access its data
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/testData.xlsx
+++ b/src/test/java/TestData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationClasses\2025\Group5-2025\SeleniumJava5thGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C0E41C-1822-456B-8045-2A7C130F8D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698DE531-05AB-4B6D-BB76-C5FB14FC31C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29985" yWindow="630" windowWidth="9480" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41835" yWindow="4620" windowWidth="14400" windowHeight="7275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Username</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>invadi@email.com</t>
-  </si>
-  <si>
-    <t>12345678</t>
   </si>
   <si>
     <t>#123ew4567dsf8w</t>
@@ -398,7 +395,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -420,15 +417,15 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
+      <c r="B3" s="4">
+        <v>12345678</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
added logic to write back to the file
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/testData.xlsx
+++ b/src/test/java/TestData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationClasses\2025\Group5-2025\SeleniumJava5thGroup2025\src\test\java\TestData\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Username</t>
   </si>
@@ -40,12 +40,16 @@
   </si>
   <si>
     <t>#123ew4567dsf8w</t>
+  </si>
+  <si>
+    <t>PasswordChanged</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -400,8 +404,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7265625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.453125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -417,7 +421,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>